<commit_message>
Se completó el proceso de descarga
</commit_message>
<xml_diff>
--- a/credenciales.xlsx
+++ b/credenciales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOS\ROBOT GRIKY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECA85CE-F591-48A1-ADEF-01C1F14C8D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D73915-BCBE-4614-8ABF-48A0014C58A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{13FC1269-D942-42AF-8CF8-8188C9792E2B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13FC1269-D942-42AF-8CF8-8188C9792E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="credenciales" sheetId="1" r:id="rId1"/>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CDDC21-BE25-4451-839A-1DB90733BDD9}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F941A4-AB0E-4F7F-B6A8-D52D3B44B0B2}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se agrega archivo main y robot para descarga de informe de usuarios
</commit_message>
<xml_diff>
--- a/credenciales.xlsx
+++ b/credenciales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOS\ROBOT GRIKY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D73915-BCBE-4614-8ABF-48A0014C58A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D423C4BC-F1C5-4A4E-8C7B-AA30B8963688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13FC1269-D942-42AF-8CF8-8188C9792E2B}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>esteban.gaviria@griky.co</t>
-  </si>
-  <si>
     <t>Griky2022!</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>Administración de Sistemas Operativos</t>
+  </si>
+  <si>
+    <t>natalia.gonzalezb@griky.co</t>
   </si>
 </sst>
 </file>
@@ -72,12 +72,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <color rgb="FF242424"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,16 +95,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CDDC21-BE25-4451-839A-1DB90733BDD9}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,7 +427,7 @@
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -438,19 +435,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{89A8827F-46A4-43CE-A747-A9A8D882EBEF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -469,17 +514,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>